<commit_message>
code returns run len of string
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3807BF2F-1690-486B-AA92-C09CAFD0E5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ACE897-71C7-4218-8091-FBA0454F15F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="217">
   <si>
     <t>Topic</t>
   </si>
@@ -634,6 +634,57 @@
   </si>
   <si>
     <t>writing code</t>
+  </si>
+  <si>
+    <t>n2 solution</t>
+  </si>
+  <si>
+    <t>need to find O(n)</t>
+  </si>
+  <si>
+    <t>discussing above code</t>
+  </si>
+  <si>
+    <t>x - 11:45</t>
+  </si>
+  <si>
+    <t>Print list items containing all characters of a given word</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/print-list-items-containing-all-characters-of-a-given-word/</t>
+  </si>
+  <si>
+    <t>11:55 - 12:40</t>
+  </si>
+  <si>
+    <t>not done, skipped</t>
+  </si>
+  <si>
+    <t>frustrated break</t>
+  </si>
+  <si>
+    <t>Strings</t>
+  </si>
+  <si>
+    <t>Reverse words in a given string</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/reverse-words-in-a-given-string/</t>
+  </si>
+  <si>
+    <t>11:28 - 12:07</t>
+  </si>
+  <si>
+    <t>Run Length Encoding</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/run-length-encoding/</t>
+  </si>
+  <si>
+    <t>headache break</t>
+  </si>
+  <si>
+    <t>1:42 - 1:53</t>
   </si>
 </sst>
 </file>
@@ -699,10 +750,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -984,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1003,14 +1054,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="6">
         <v>44011</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" t="s">
         <v>38</v>
       </c>
@@ -1241,13 +1292,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>44012</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18">
@@ -1517,13 +1568,13 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C39" s="5">
+      <c r="C39" s="6">
         <v>44013</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B40">
@@ -1677,12 +1728,12 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C54" s="5">
+      <c r="C54" s="6">
         <v>44014</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B55">
@@ -1811,12 +1862,12 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C67" s="5">
+      <c r="C67" s="6">
         <v>44015</v>
       </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D68" t="s">
@@ -1949,7 +2000,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>158</v>
       </c>
@@ -1957,8 +2008,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="6" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>185</v>
       </c>
       <c r="B82" t="s">
@@ -1971,7 +2022,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D83" t="s">
         <v>188</v>
       </c>
@@ -1979,7 +2030,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>160</v>
       </c>
@@ -1990,7 +2041,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D85" t="s">
         <v>90</v>
       </c>
@@ -1998,7 +2049,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>160</v>
       </c>
@@ -2012,7 +2063,10 @@
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="B87" t="s">
         <v>160</v>
       </c>
@@ -2023,7 +2077,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D88" t="s">
         <v>133</v>
       </c>
@@ -2031,7 +2085,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D89" t="s">
         <v>133</v>
       </c>
@@ -2039,12 +2093,86 @@
         <v>197</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C90" t="s">
         <v>199</v>
       </c>
       <c r="E90" t="s">
         <v>198</v>
+      </c>
+      <c r="F90" t="s">
+        <v>200</v>
+      </c>
+      <c r="G90" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C91" t="s">
+        <v>202</v>
+      </c>
+      <c r="E91" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" t="s">
+        <v>160</v>
+      </c>
+      <c r="C92" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" t="s">
+        <v>207</v>
+      </c>
+      <c r="E92" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D93" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B94" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" t="s">
+        <v>79</v>
+      </c>
+      <c r="E94" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B95" t="s">
+        <v>160</v>
+      </c>
+      <c r="C95" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D96" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E97" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2057,9 +2185,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A82" r:id="rId1" xr:uid="{3CD2EBDC-89BA-47DB-A719-9C8261C9249C}"/>
+    <hyperlink ref="A92" r:id="rId2" xr:uid="{977D6760-AE76-4AB0-89D0-8667F36F6EB6}"/>
+    <hyperlink ref="A94" r:id="rId3" xr:uid="{F0EE4017-BF97-46B2-A92E-0DB245C3A136}"/>
+    <hyperlink ref="A95" r:id="rId4" xr:uid="{BA6E722D-BB9C-46C7-9A65-878781566886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
turn of kth bit from right
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265099D9-43AA-4518-B672-FEF2E967B2B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CBAAC-2110-423F-B0B9-EC50DB0AA9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="239">
   <si>
     <t>Topic</t>
   </si>
@@ -703,6 +703,54 @@
   </si>
   <si>
     <t>coding</t>
+  </si>
+  <si>
+    <t>done 1 error in logical or and</t>
+  </si>
+  <si>
+    <t>x - 3:10</t>
+  </si>
+  <si>
+    <t>coded and tested</t>
+  </si>
+  <si>
+    <t>How to turn off a particular bit in a number?</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/how-to-turn-off-a-particular-bit-in-a-number/</t>
+  </si>
+  <si>
+    <t>3:22 - 3:37</t>
+  </si>
+  <si>
+    <t>x - 3:42</t>
+  </si>
+  <si>
+    <t>Find Excel column name from a given column number</t>
+  </si>
+  <si>
+    <t>3:56 - 4:13</t>
+  </si>
+  <si>
+    <t>Program to print all palindromes in a given range</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/program-print-palindromes-given-range/</t>
+  </si>
+  <si>
+    <t>4:19 - 4:34</t>
+  </si>
+  <si>
+    <t>done brute force</t>
+  </si>
+  <si>
+    <t>Print all pairs of anagrams in a given array of strings</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/print-pairs-anagrams-given-array-strings/</t>
+  </si>
+  <si>
+    <t>4:49 - 5:22</t>
   </si>
 </sst>
 </file>
@@ -1053,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2225,12 +2273,81 @@
       <c r="C100" t="s">
         <v>219</v>
       </c>
+      <c r="D100" t="s">
+        <v>223</v>
+      </c>
       <c r="E100" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D101" t="s">
+        <v>225</v>
+      </c>
+      <c r="E101" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C102" t="s">
+        <v>226</v>
+      </c>
+      <c r="D102" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D103" t="s">
+        <v>217</v>
+      </c>
+      <c r="E103" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>230</v>
+      </c>
+      <c r="D104" t="s">
+        <v>128</v>
+      </c>
+      <c r="E104" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C105" t="s">
+        <v>232</v>
+      </c>
+      <c r="D105" t="s">
+        <v>235</v>
+      </c>
+      <c r="E105" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" t="s">
+        <v>236</v>
+      </c>
+      <c r="E106" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D107" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2249,9 +2366,12 @@
     <hyperlink ref="A95" r:id="rId3" xr:uid="{F0EE4017-BF97-46B2-A92E-0DB245C3A136}"/>
     <hyperlink ref="A96" r:id="rId4" xr:uid="{BA6E722D-BB9C-46C7-9A65-878781566886}"/>
     <hyperlink ref="A100" r:id="rId5" xr:uid="{FD79C6AB-C39B-4D06-860C-A1D68EFF7D0E}"/>
+    <hyperlink ref="A102" r:id="rId6" xr:uid="{156F719D-0B61-472C-AC56-0E409862052B}"/>
+    <hyperlink ref="A105" r:id="rId7" xr:uid="{491FA8EF-FC74-4665-BEE5-809133E670FC}"/>
+    <hyperlink ref="A106" r:id="rId8" xr:uid="{4E4DBC57-1E81-4A08-BE61-86EEB321A9C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
prints pairs of anagrams from given list of words
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CBAAC-2110-423F-B0B9-EC50DB0AA9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB28B23-DE0E-4683-AF64-DF5086924AE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="246">
   <si>
     <t>Topic</t>
   </si>
@@ -751,6 +751,27 @@
   </si>
   <si>
     <t>4:49 - 5:22</t>
+  </si>
+  <si>
+    <t>5:23 - x</t>
+  </si>
+  <si>
+    <t>done 1 error, sorting strings</t>
+  </si>
+  <si>
+    <t>tea break</t>
+  </si>
+  <si>
+    <t>x - 6:18</t>
+  </si>
+  <si>
+    <t>Check if characters of a given string can be rearranged to form a palindrome</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/check-characters-given-string-can-rearranged-form-palindrome/</t>
+  </si>
+  <si>
+    <t>6:25 - x</t>
   </si>
 </sst>
 </file>
@@ -1101,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2270,6 +2291,9 @@
       <c r="A100" s="5" t="s">
         <v>220</v>
       </c>
+      <c r="B100" t="s">
+        <v>160</v>
+      </c>
       <c r="C100" t="s">
         <v>219</v>
       </c>
@@ -2292,6 +2316,9 @@
       <c r="A102" s="5" t="s">
         <v>227</v>
       </c>
+      <c r="B102" t="s">
+        <v>160</v>
+      </c>
       <c r="C102" t="s">
         <v>226</v>
       </c>
@@ -2311,6 +2338,9 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B104" t="s">
+        <v>160</v>
+      </c>
       <c r="C104" t="s">
         <v>230</v>
       </c>
@@ -2325,6 +2355,9 @@
       <c r="A105" s="5" t="s">
         <v>233</v>
       </c>
+      <c r="B105" t="s">
+        <v>160</v>
+      </c>
       <c r="C105" t="s">
         <v>232</v>
       </c>
@@ -2339,8 +2372,14 @@
       <c r="A106" s="5" t="s">
         <v>237</v>
       </c>
+      <c r="B106" t="s">
+        <v>160</v>
+      </c>
       <c r="C106" t="s">
         <v>236</v>
+      </c>
+      <c r="D106" t="s">
+        <v>240</v>
       </c>
       <c r="E106" t="s">
         <v>238</v>
@@ -2349,6 +2388,28 @@
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D107" t="s">
         <v>222</v>
+      </c>
+      <c r="E107" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D108" t="s">
+        <v>241</v>
+      </c>
+      <c r="E108" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C109" t="s">
+        <v>243</v>
+      </c>
+      <c r="E109" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2369,9 +2430,10 @@
     <hyperlink ref="A102" r:id="rId6" xr:uid="{156F719D-0B61-472C-AC56-0E409862052B}"/>
     <hyperlink ref="A105" r:id="rId7" xr:uid="{491FA8EF-FC74-4665-BEE5-809133E670FC}"/>
     <hyperlink ref="A106" r:id="rId8" xr:uid="{4E4DBC57-1E81-4A08-BE61-86EEB321A9C8}"/>
+    <hyperlink ref="A109" r:id="rId9" xr:uid="{4A2B4B63-4B0B-4599-BE00-06886FA09C69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check if word can made a plaindrome by rearranging
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB28B23-DE0E-4683-AF64-DF5086924AE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE4EB7A-ABED-4791-B5AE-5C8561796628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="251">
   <si>
     <t>Topic</t>
   </si>
@@ -772,6 +772,21 @@
   </si>
   <si>
     <t>6:25 - x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 6:44</t>
+  </si>
+  <si>
+    <t>x - 7:15</t>
+  </si>
+  <si>
+    <t>Given two strings, find if first string is a subsequence of second</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/given-two-strings-find-first-string-subsequence-second/</t>
+  </si>
+  <si>
+    <t>7:25 - 7:43</t>
   </si>
 </sst>
 </file>
@@ -1122,17 +1137,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.90625" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
@@ -2405,11 +2421,52 @@
       <c r="A109" s="5" t="s">
         <v>244</v>
       </c>
+      <c r="B109" t="s">
+        <v>160</v>
+      </c>
       <c r="C109" t="s">
         <v>243</v>
       </c>
+      <c r="D109" t="s">
+        <v>5</v>
+      </c>
       <c r="E109" t="s">
         <v>245</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D110" t="s">
+        <v>217</v>
+      </c>
+      <c r="E110" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D111" t="s">
+        <v>65</v>
+      </c>
+      <c r="E111" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B112" t="s">
+        <v>160</v>
+      </c>
+      <c r="C112" t="s">
+        <v>248</v>
+      </c>
+      <c r="E112" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D113" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2431,9 +2488,10 @@
     <hyperlink ref="A105" r:id="rId7" xr:uid="{491FA8EF-FC74-4665-BEE5-809133E670FC}"/>
     <hyperlink ref="A106" r:id="rId8" xr:uid="{4E4DBC57-1E81-4A08-BE61-86EEB321A9C8}"/>
     <hyperlink ref="A109" r:id="rId9" xr:uid="{4A2B4B63-4B0B-4599-BE00-06886FA09C69}"/>
+    <hyperlink ref="A112" r:id="rId10" xr:uid="{1A7D1F9C-4239-4431-8158-67B11673D23F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GFG_ max depth of nested parenthesis string
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE4EB7A-ABED-4791-B5AE-5C8561796628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15783692-3BC5-4CDB-82F8-BEA59D0486E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="256">
   <si>
     <t>Topic</t>
   </si>
@@ -787,6 +787,21 @@
   </si>
   <si>
     <t>7:25 - 7:43</t>
+  </si>
+  <si>
+    <t>7:43 - 7:48</t>
+  </si>
+  <si>
+    <t>Find maximum depth of nested parenthesis in a string</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-maximum-depth-nested-parenthesis-string/</t>
+  </si>
+  <si>
+    <t>7:54 - 8:03</t>
+  </si>
+  <si>
+    <t>8:03 - 8:08</t>
   </si>
 </sst>
 </file>
@@ -1137,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2460,13 +2475,44 @@
       <c r="C112" t="s">
         <v>248</v>
       </c>
+      <c r="D112" t="s">
+        <v>5</v>
+      </c>
       <c r="E112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D113" t="s">
         <v>222</v>
+      </c>
+      <c r="E113" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B114" t="s">
+        <v>160</v>
+      </c>
+      <c r="C114" t="s">
+        <v>252</v>
+      </c>
+      <c r="D114" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D115" t="s">
+        <v>222</v>
+      </c>
+      <c r="E115" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2489,9 +2535,10 @@
     <hyperlink ref="A106" r:id="rId8" xr:uid="{4E4DBC57-1E81-4A08-BE61-86EEB321A9C8}"/>
     <hyperlink ref="A109" r:id="rId9" xr:uid="{4A2B4B63-4B0B-4599-BE00-06886FA09C69}"/>
     <hyperlink ref="A112" r:id="rId10" xr:uid="{1A7D1F9C-4239-4431-8158-67B11673D23F}"/>
+    <hyperlink ref="A114" r:id="rId11" xr:uid="{CC909328-F849-4F78-863E-D08127ADC5BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added a better approach with TC:O(n) and SC:O(1)
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15783692-3BC5-4CDB-82F8-BEA59D0486E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A455BC83-7E54-4CD5-9DE8-97E709C3C13B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="259">
   <si>
     <t>Topic</t>
   </si>
@@ -802,6 +802,15 @@
   </si>
   <si>
     <t>8:03 - 8:08</t>
+  </si>
+  <si>
+    <t>done, using stack, better method exists</t>
+  </si>
+  <si>
+    <t>doing better method without SC O(n)</t>
+  </si>
+  <si>
+    <t>8:11 - x</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A110" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2501,7 +2510,7 @@
         <v>252</v>
       </c>
       <c r="D114" t="s">
-        <v>5</v>
+        <v>256</v>
       </c>
       <c r="E114" t="s">
         <v>254</v>
@@ -2513,6 +2522,14 @@
       </c>
       <c r="E115" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D116" t="s">
+        <v>257</v>
+      </c>
+      <c r="E116" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GFG _ get excel column name from column num
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A455BC83-7E54-4CD5-9DE8-97E709C3C13B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0CA13-4553-48F0-86C4-2AD0E726EEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="260">
   <si>
     <t>Topic</t>
   </si>
@@ -810,7 +810,10 @@
     <t>doing better method without SC O(n)</t>
   </si>
   <si>
-    <t>8:11 - x</t>
+    <t>8:11 - 8:17</t>
+  </si>
+  <si>
+    <t>8:23 - x</t>
   </si>
 </sst>
 </file>
@@ -1161,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2530,6 +2533,14 @@
       </c>
       <c r="E116" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D117" t="s">
+        <v>158</v>
+      </c>
+      <c r="E117" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
k rotate array to the left
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0CA13-4553-48F0-86C4-2AD0E726EEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98AA7D5-86BC-4177-85D0-F63E505945F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="295">
   <si>
     <t>Topic</t>
   </si>
@@ -814,6 +814,111 @@
   </si>
   <si>
     <t>8:23 - x</t>
+  </si>
+  <si>
+    <t>applying dinner</t>
+  </si>
+  <si>
+    <t>11:45 - x</t>
+  </si>
+  <si>
+    <t>doing excel column name</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/majority-element/</t>
+  </si>
+  <si>
+    <t>12:50- 1:19</t>
+  </si>
+  <si>
+    <t>Largest Sum Contiguous Subarray</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/largest-sum-contiguous-subarray/</t>
+  </si>
+  <si>
+    <t>1;22 -1:37</t>
+  </si>
+  <si>
+    <t>x - 2:23</t>
+  </si>
+  <si>
+    <t>brunch break</t>
+  </si>
+  <si>
+    <t>60+40</t>
+  </si>
+  <si>
+    <t>1st iter</t>
+  </si>
+  <si>
+    <t>2/6</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>2/5</t>
+  </si>
+  <si>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>1/5</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>x - 3:39</t>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>3/6</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>6/12</t>
+  </si>
+  <si>
+    <t>Merge an array of size n into another array of size m+n</t>
+  </si>
+  <si>
+    <t>3:40 - 4:18</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/merge-one-array-of-size-n-into-another-one-of-size-mn/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/array-rotation/</t>
+  </si>
+  <si>
+    <t>Program for array rotation</t>
+  </si>
+  <si>
+    <t>4:34 -4:48</t>
+  </si>
+  <si>
+    <t>x - 4:53</t>
+  </si>
+  <si>
+    <t>Two elements whose sum is closest to zero</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/two-elements-whose-sum-is-closest-to-zero/</t>
+  </si>
+  <si>
+    <t>5:00 - x</t>
   </si>
 </sst>
 </file>
@@ -873,7 +978,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -881,6 +986,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1164,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1693,6 +1803,9 @@
       <c r="C38" t="s">
         <v>96</v>
       </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
       <c r="F38" s="2" t="s">
         <v>97</v>
       </c>
@@ -2309,12 +2422,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D97" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D98" t="s">
         <v>5</v>
       </c>
@@ -2322,7 +2435,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D99" t="s">
         <v>217</v>
       </c>
@@ -2330,7 +2443,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>220</v>
       </c>
@@ -2346,8 +2459,11 @@
       <c r="E100" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D101" t="s">
         <v>225</v>
       </c>
@@ -2355,7 +2471,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>227</v>
       </c>
@@ -2372,7 +2488,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D103" t="s">
         <v>217</v>
       </c>
@@ -2380,7 +2496,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>160</v>
       </c>
@@ -2394,7 +2510,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>233</v>
       </c>
@@ -2411,7 +2527,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>237</v>
       </c>
@@ -2428,7 +2544,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D107" t="s">
         <v>222</v>
       </c>
@@ -2436,7 +2552,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D108" t="s">
         <v>241</v>
       </c>
@@ -2444,7 +2560,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>244</v>
       </c>
@@ -2461,7 +2577,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D110" t="s">
         <v>217</v>
       </c>
@@ -2469,7 +2585,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D111" t="s">
         <v>65</v>
       </c>
@@ -2477,7 +2593,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>249</v>
       </c>
@@ -2494,7 +2610,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D113" t="s">
         <v>222</v>
       </c>
@@ -2502,7 +2618,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>253</v>
       </c>
@@ -2519,7 +2635,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D115" t="s">
         <v>222</v>
       </c>
@@ -2527,7 +2643,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D116" t="s">
         <v>257</v>
       </c>
@@ -2535,16 +2651,136 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D117" t="s">
-        <v>158</v>
+        <v>260</v>
       </c>
       <c r="E117" t="s">
         <v>259</v>
       </c>
     </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C118" t="s">
+        <v>262</v>
+      </c>
+      <c r="D118" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="6">
+        <v>44017</v>
+      </c>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B120" t="s">
+        <v>160</v>
+      </c>
+      <c r="C120" t="s">
+        <v>263</v>
+      </c>
+      <c r="E120" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B121" t="s">
+        <v>160</v>
+      </c>
+      <c r="C121" t="s">
+        <v>266</v>
+      </c>
+      <c r="E121" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D122" t="s">
+        <v>270</v>
+      </c>
+      <c r="E122" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D123" t="s">
+        <v>278</v>
+      </c>
+      <c r="E123" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B124" t="s">
+        <v>160</v>
+      </c>
+      <c r="C124" t="s">
+        <v>285</v>
+      </c>
+      <c r="D124" t="s">
+        <v>79</v>
+      </c>
+      <c r="E124" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B125" t="s">
+        <v>160</v>
+      </c>
+      <c r="C125" t="s">
+        <v>289</v>
+      </c>
+      <c r="D125" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D126" t="s">
+        <v>222</v>
+      </c>
+      <c r="E126" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B127" t="s">
+        <v>160</v>
+      </c>
+      <c r="C127" t="s">
+        <v>292</v>
+      </c>
+      <c r="E127" t="s">
+        <v>294</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C119:F119"/>
     <mergeCell ref="C94:F94"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="C17:G17"/>
@@ -2564,49 +2800,181 @@
     <hyperlink ref="A109" r:id="rId9" xr:uid="{4A2B4B63-4B0B-4599-BE00-06886FA09C69}"/>
     <hyperlink ref="A112" r:id="rId10" xr:uid="{1A7D1F9C-4239-4431-8158-67B11673D23F}"/>
     <hyperlink ref="A114" r:id="rId11" xr:uid="{CC909328-F849-4F78-863E-D08127ADC5BF}"/>
+    <hyperlink ref="A120" r:id="rId12" xr:uid="{C16E7A3A-2A29-4986-A7DE-3FA88A27C473}"/>
+    <hyperlink ref="A121" r:id="rId13" xr:uid="{2DEACBF7-B810-4789-9BBA-F5CE5E7F5C31}"/>
+    <hyperlink ref="A124" r:id="rId14" xr:uid="{80AE93BD-E236-4B9D-B1F9-5A2291065BF1}"/>
+    <hyperlink ref="A125" r:id="rId15" xr:uid="{06DA1B4B-4D96-4AF1-BF91-5D1255E063F4}"/>
+    <hyperlink ref="A127" r:id="rId16" xr:uid="{D474E2DD-F72B-47E9-B277-9AA846384A68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64DFDFF5-44B9-44D8-9FB0-A773253A1BED}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="172" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="172" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.90625" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C1" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>123</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
get pair with its sum closest to zero
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98AA7D5-86BC-4177-85D0-F63E505945F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FA580F-B94E-4243-A87E-94797F8942A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="307">
   <si>
     <t>Topic</t>
   </si>
@@ -840,9 +840,6 @@
     <t>https://www.geeksforgeeks.org/largest-sum-contiguous-subarray/</t>
   </si>
   <si>
-    <t>1;22 -1:37</t>
-  </si>
-  <si>
     <t>x - 2:23</t>
   </si>
   <si>
@@ -918,7 +915,46 @@
     <t>https://www.geeksforgeeks.org/two-elements-whose-sum-is-closest-to-zero/</t>
   </si>
   <si>
-    <t>5:00 - x</t>
+    <t>5:00 - 5:18</t>
+  </si>
+  <si>
+    <t>coding, doesn't work</t>
+  </si>
+  <si>
+    <t>x - 5:22</t>
+  </si>
+  <si>
+    <t>1:22 -1:37</t>
+  </si>
+  <si>
+    <t>Check for Majority Element in a sorted array</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/check-for-majority-element-in-a-sorted-array/</t>
+  </si>
+  <si>
+    <t>5:32- 5:55</t>
+  </si>
+  <si>
+    <t>O(logn) not done, O(n) approach done</t>
+  </si>
+  <si>
+    <t>Given only a pointer/reference to a node to be deleted in a singly linked list, how do you delete it?</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/given-only-a-pointer-to-a-node-to-be-deleted-in-a-singly-linked-list-how-do-you-delete-it/</t>
+  </si>
+  <si>
+    <t>6:04 - 6:19</t>
+  </si>
+  <si>
+    <t>Detect loop in a linked list</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/detect-loop-in-a-linked-list/</t>
+  </si>
+  <si>
+    <t>6:21 - x</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2460,7 +2496,7 @@
         <v>221</v>
       </c>
       <c r="F100" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -2688,6 +2724,9 @@
       <c r="C120" t="s">
         <v>263</v>
       </c>
+      <c r="D120" t="s">
+        <v>5</v>
+      </c>
       <c r="E120" t="s">
         <v>265</v>
       </c>
@@ -2702,58 +2741,61 @@
       <c r="C121" t="s">
         <v>266</v>
       </c>
+      <c r="D121" t="s">
+        <v>5</v>
+      </c>
       <c r="E121" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D122" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E122" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D123" t="s">
+        <v>277</v>
+      </c>
+      <c r="E123" t="s">
         <v>278</v>
-      </c>
-      <c r="E123" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B124" t="s">
         <v>160</v>
       </c>
       <c r="C124" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D124" t="s">
         <v>79</v>
       </c>
       <c r="E124" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B125" t="s">
         <v>160</v>
       </c>
       <c r="C125" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D125" t="s">
         <v>5</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
@@ -2761,21 +2803,77 @@
         <v>222</v>
       </c>
       <c r="E126" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B127" t="s">
         <v>160</v>
       </c>
       <c r="C127" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="D127" t="s">
+        <v>176</v>
       </c>
       <c r="E127" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D128" t="s">
         <v>294</v>
+      </c>
+      <c r="E128" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B129" t="s">
+        <v>160</v>
+      </c>
+      <c r="C129" t="s">
+        <v>297</v>
+      </c>
+      <c r="D129" t="s">
+        <v>300</v>
+      </c>
+      <c r="E129" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C130" t="s">
+        <v>301</v>
+      </c>
+      <c r="E130" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B131" t="s">
+        <v>160</v>
+      </c>
+      <c r="C131" t="s">
+        <v>304</v>
+      </c>
+      <c r="E131" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2805,9 +2903,12 @@
     <hyperlink ref="A124" r:id="rId14" xr:uid="{80AE93BD-E236-4B9D-B1F9-5A2291065BF1}"/>
     <hyperlink ref="A125" r:id="rId15" xr:uid="{06DA1B4B-4D96-4AF1-BF91-5D1255E063F4}"/>
     <hyperlink ref="A127" r:id="rId16" xr:uid="{D474E2DD-F72B-47E9-B277-9AA846384A68}"/>
+    <hyperlink ref="A129" r:id="rId17" xr:uid="{90FAA65B-DF0B-4C06-91A5-952C60A68AB9}"/>
+    <hyperlink ref="B130" r:id="rId18" xr:uid="{C94CD290-86AE-4102-A5BD-49DE426A9829}"/>
+    <hyperlink ref="A131" r:id="rId19" xr:uid="{165A41A5-618D-4838-9941-E82584D9FD0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2815,7 +2916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64DFDFF5-44B9-44D8-9FB0-A773253A1BED}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="172" workbookViewId="0">
+    <sheetView zoomScale="172" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2832,7 +2933,7 @@
         <v>119</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="1"/>
@@ -2846,7 +2947,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D2" s="8">
         <v>0.8</v>
@@ -2854,10 +2955,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D3" s="8">
         <v>0.8</v>
@@ -2871,7 +2972,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D4" s="8">
         <v>0.4</v>
@@ -2885,7 +2986,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D5" s="8">
         <v>0.5</v>
@@ -2899,7 +3000,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D6" s="8">
         <v>0.2</v>
@@ -2910,7 +3011,7 @@
         <v>74</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="8">
         <v>0.33333333333333331</v>
@@ -2921,7 +3022,7 @@
         <v>108</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D8" s="8">
         <v>0.33333333333333331</v>
@@ -2932,7 +3033,7 @@
         <v>124</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" s="8">
         <v>0.4</v>
@@ -2943,7 +3044,7 @@
         <v>142</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D10" s="8">
         <v>0.5</v>
@@ -2954,7 +3055,7 @@
         <v>168</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D11" s="8">
         <v>0.6</v>
@@ -2965,7 +3066,7 @@
         <v>209</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D12" s="8">
         <v>0.5</v>

</xml_diff>

<commit_message>
remove repeated digits in a given integer
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FA580F-B94E-4243-A87E-94797F8942A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4014483F-7583-488A-9BEB-58887EC0F074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="329">
   <si>
     <t>Topic</t>
   </si>
@@ -954,7 +954,73 @@
     <t>https://www.geeksforgeeks.org/detect-loop-in-a-linked-list/</t>
   </si>
   <si>
-    <t>6:21 - x</t>
+    <t>6:21 - 6:30</t>
+  </si>
+  <si>
+    <t>6:30 - 35</t>
+  </si>
+  <si>
+    <t>Reverse a Doubly Linked List</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/reverse-a-doubly-linked-list/</t>
+  </si>
+  <si>
+    <t>6:40 - 6:49</t>
+  </si>
+  <si>
+    <t>x-7:35</t>
+  </si>
+  <si>
+    <t>Split a Circular Linked List into two halves</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/split-a-circular-linked-list-into-two-halves/</t>
+  </si>
+  <si>
+    <t>7:43 - 8:02</t>
+  </si>
+  <si>
+    <t>Intersection of two Sorted Linked Lists</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/intersection-of-two-sorted-linked-lists/</t>
+  </si>
+  <si>
+    <t>8:07 - 8:16</t>
+  </si>
+  <si>
+    <t>2nd iter</t>
+  </si>
+  <si>
+    <t>5/5</t>
+  </si>
+  <si>
+    <t>Find the nearest smaller numbers on left side in an array</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-the-nearest-smaller-numbers-on-left-side-in-an-array/</t>
+  </si>
+  <si>
+    <t>Stacks</t>
+  </si>
+  <si>
+    <t>8:34 - 8:45</t>
+  </si>
+  <si>
+    <t>x - 11:49</t>
+  </si>
+  <si>
+    <t>Remove repeated digits in a given number</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/remove-repeated-digits-in-a-given-number/</t>
+  </si>
+  <si>
+    <t>11:50 - 12:04</t>
+  </si>
+  <si>
+    <t>x - 12:08</t>
   </si>
 </sst>
 </file>
@@ -1021,11 +1087,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1310,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1324,20 +1390,23 @@
     <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="6.08984375" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="3.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="8">
         <v>44011</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" t="s">
         <v>38</v>
       </c>
@@ -1568,13 +1637,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="6">
+      <c r="C17" s="8">
         <v>44012</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18">
@@ -1847,13 +1916,13 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C39" s="6">
+      <c r="C39" s="8">
         <v>44013</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B40">
@@ -2007,12 +2076,12 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C54" s="6">
+      <c r="C54" s="8">
         <v>44014</v>
       </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B55">
@@ -2141,12 +2210,12 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C67" s="6">
+      <c r="C67" s="8">
         <v>44015</v>
       </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D68" t="s">
@@ -2420,12 +2489,12 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C94" s="6">
+      <c r="C94" s="8">
         <v>44016</v>
       </c>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
@@ -2707,12 +2776,12 @@
       <c r="A119" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C119" s="6">
+      <c r="C119" s="8">
         <v>44017</v>
       </c>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
-      <c r="F119" s="6"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
@@ -2831,7 +2900,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>298</v>
       </c>
@@ -2848,21 +2917,27 @@
         <v>299</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B130" s="5" t="s">
-        <v>302</v>
+      <c r="B130" t="s">
+        <v>160</v>
       </c>
       <c r="C130" t="s">
         <v>301</v>
       </c>
+      <c r="D130" t="s">
+        <v>5</v>
+      </c>
       <c r="E130" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F130" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>305</v>
       </c>
@@ -2872,8 +2947,139 @@
       <c r="C131" t="s">
         <v>304</v>
       </c>
+      <c r="D131" t="s">
+        <v>5</v>
+      </c>
       <c r="E131" t="s">
         <v>306</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D132" t="s">
+        <v>222</v>
+      </c>
+      <c r="E132" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B133" t="s">
+        <v>160</v>
+      </c>
+      <c r="C133" t="s">
+        <v>308</v>
+      </c>
+      <c r="D133" t="s">
+        <v>5</v>
+      </c>
+      <c r="E133" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D134" t="s">
+        <v>65</v>
+      </c>
+      <c r="E134" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B135" t="s">
+        <v>160</v>
+      </c>
+      <c r="C135" t="s">
+        <v>312</v>
+      </c>
+      <c r="D135" t="s">
+        <v>5</v>
+      </c>
+      <c r="E135" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B136" t="s">
+        <v>160</v>
+      </c>
+      <c r="C136" t="s">
+        <v>315</v>
+      </c>
+      <c r="D136" t="s">
+        <v>5</v>
+      </c>
+      <c r="E136" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B137" t="s">
+        <v>160</v>
+      </c>
+      <c r="C137" t="s">
+        <v>320</v>
+      </c>
+      <c r="D137" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137" t="s">
+        <v>323</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D138" t="s">
+        <v>90</v>
+      </c>
+      <c r="E138" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D139" t="s">
+        <v>158</v>
+      </c>
+      <c r="E139" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B140" t="s">
+        <v>160</v>
+      </c>
+      <c r="C140" t="s">
+        <v>325</v>
+      </c>
+      <c r="D140" t="s">
+        <v>5</v>
+      </c>
+      <c r="E140" t="s">
+        <v>327</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D141" t="s">
+        <v>217</v>
+      </c>
+      <c r="E141" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2904,11 +3110,16 @@
     <hyperlink ref="A125" r:id="rId15" xr:uid="{06DA1B4B-4D96-4AF1-BF91-5D1255E063F4}"/>
     <hyperlink ref="A127" r:id="rId16" xr:uid="{D474E2DD-F72B-47E9-B277-9AA846384A68}"/>
     <hyperlink ref="A129" r:id="rId17" xr:uid="{90FAA65B-DF0B-4C06-91A5-952C60A68AB9}"/>
-    <hyperlink ref="B130" r:id="rId18" xr:uid="{C94CD290-86AE-4102-A5BD-49DE426A9829}"/>
+    <hyperlink ref="F130" r:id="rId18" xr:uid="{C94CD290-86AE-4102-A5BD-49DE426A9829}"/>
     <hyperlink ref="A131" r:id="rId19" xr:uid="{165A41A5-618D-4838-9941-E82584D9FD0D}"/>
+    <hyperlink ref="A133" r:id="rId20" xr:uid="{ED09429E-35E8-4073-ADDB-3C1DDB0FC0A7}"/>
+    <hyperlink ref="A135" r:id="rId21" xr:uid="{F01C5FFE-48FA-4A66-84D9-E03556ADDBFB}"/>
+    <hyperlink ref="A136" r:id="rId22" xr:uid="{CFBBC7F9-98D1-4531-A1AF-BB1CBB832277}"/>
+    <hyperlink ref="F137" r:id="rId23" xr:uid="{5B58A089-4079-49A4-BA43-492ABDDA68D5}"/>
+    <hyperlink ref="F140" r:id="rId24" xr:uid="{F4A67570-1C26-4133-A95C-EC6BA04F4ECD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -2917,14 +3128,14 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="172" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.26953125" customWidth="1"/>
     <col min="2" max="2" width="12.36328125" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2936,7 +3147,9 @@
         <v>271</v>
       </c>
       <c r="D1" s="9"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2946,23 +3159,31 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>0.8</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.8</v>
       </c>
+      <c r="E3" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -2971,12 +3192,14 @@
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0.4</v>
       </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -2985,12 +3208,14 @@
       <c r="B5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>0.5</v>
       </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -2999,78 +3224,92 @@
       <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>0.2</v>
       </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0.33333333333333331</v>
       </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.33333333333333331</v>
       </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>0.4</v>
       </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>0.5</v>
       </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>0.6</v>
       </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>0.5</v>
       </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
return max possible sum equal in 3 stacks
</commit_message>
<xml_diff>
--- a/session4/Score_iterations.xlsx
+++ b/session4/Score_iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4014483F-7583-488A-9BEB-58887EC0F074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B47E01-C3B2-4C13-B65C-848756B8FAC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="340">
   <si>
     <t>Topic</t>
   </si>
@@ -1021,6 +1021,39 @@
   </si>
   <si>
     <t>x - 12:08</t>
+  </si>
+  <si>
+    <t>Find if an expression has duplicate parenthesis or not</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-expression-duplicate-parenthesis-not/</t>
+  </si>
+  <si>
+    <t>12:20 - 12:50</t>
+  </si>
+  <si>
+    <t>Find maximum sum possible equal sum of three stacks</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-maximum-sum-possible-equal-sum-three-stacks/</t>
+  </si>
+  <si>
+    <t>1:07 - 1:29</t>
+  </si>
+  <si>
+    <t>x - 1:58</t>
+  </si>
+  <si>
+    <t>done 1 logical comparision error</t>
+  </si>
+  <si>
+    <t>Sort a stack using a temporary stack</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/sort-stack-using-temporary-stack/</t>
+  </si>
+  <si>
+    <t>12:07 - 12:30</t>
   </si>
 </sst>
 </file>
@@ -1376,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3080,6 +3113,62 @@
       </c>
       <c r="E141" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B142" t="s">
+        <v>160</v>
+      </c>
+      <c r="C142" t="s">
+        <v>329</v>
+      </c>
+      <c r="D142" t="s">
+        <v>79</v>
+      </c>
+      <c r="E142" t="s">
+        <v>331</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B143" t="s">
+        <v>160</v>
+      </c>
+      <c r="C143" t="s">
+        <v>332</v>
+      </c>
+      <c r="D143" t="s">
+        <v>336</v>
+      </c>
+      <c r="E143" t="s">
+        <v>334</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D144" t="s">
+        <v>222</v>
+      </c>
+      <c r="E144" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B145" t="s">
+        <v>160</v>
+      </c>
+      <c r="C145" t="s">
+        <v>337</v>
+      </c>
+      <c r="E145" t="s">
+        <v>339</v>
+      </c>
+      <c r="F145" s="5" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3117,9 +3206,12 @@
     <hyperlink ref="A136" r:id="rId22" xr:uid="{CFBBC7F9-98D1-4531-A1AF-BB1CBB832277}"/>
     <hyperlink ref="F137" r:id="rId23" xr:uid="{5B58A089-4079-49A4-BA43-492ABDDA68D5}"/>
     <hyperlink ref="F140" r:id="rId24" xr:uid="{F4A67570-1C26-4133-A95C-EC6BA04F4ECD}"/>
+    <hyperlink ref="F142" r:id="rId25" xr:uid="{189B0DB9-4C79-46CC-92C7-5190530925F9}"/>
+    <hyperlink ref="F143" r:id="rId26" xr:uid="{ADC3A20C-F06E-43CA-83ED-EF5948163080}"/>
+    <hyperlink ref="F145" r:id="rId27" xr:uid="{06403138-9CFA-4250-A3D4-27D157C81FA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>